<commit_message>
Removed the need for for "foundMesh" (old "reachedFaces"): New mesh is only created if 'g' is declared and when finalize is reached. New instance of RawMesh is no longer needed. Object is reset. Allow negative face indices.
</commit_message>
<xml_diff>
--- a/resource/obj/verify/CubeBuilder.xlsx
+++ b/resource/obj/verify/CubeBuilder.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\WWOBJLoader\resource\obj\cubes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\github\WWOBJLoader\resource\obj\verify\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27300" windowHeight="19980" xr2:uid="{01B4FE21-4BF6-4362-B9A5-51E441DC053B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="FaceIndexReverse" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,18 +24,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>v</t>
   </si>
   <si>
-    <t>Faktor</t>
-  </si>
-  <si>
     <t>Offset</t>
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Offset X</t>
+  </si>
+  <si>
+    <t>Offset Z</t>
+  </si>
+  <si>
+    <t>Offset Y</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>FaceIndexReverse</t>
+  </si>
+  <si>
+    <t>usemtl</t>
+  </si>
+  <si>
+    <t>red</t>
   </si>
 </sst>
 </file>
@@ -82,12 +103,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -402,19 +425,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1167990C-1D40-46E2-AB4F-08FAFAE33399}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="I1:M6"/>
+      <selection activeCell="H11" sqref="H11:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11.42578125" style="1"/>
-    <col min="7" max="7" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="11.42578125" style="6"/>
+    <col min="3" max="3" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="1.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.140625" style="3" customWidth="1"/>
     <col min="11" max="11" width="3.28515625" style="3" customWidth="1"/>
@@ -423,276 +448,375 @@
     <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="6">
         <f>-1*B1+B2</f>
         <v>40</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="6">
+        <f>1*B1+B3</f>
+        <v>10</v>
+      </c>
+      <c r="F1" s="6">
+        <f>1*B1+B4</f>
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f>CONCATENATE(C1," ",D1," ",E1," ",F1)</f>
+        <v>v 40 10 10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5">
+        <v>50</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <f>-1*B1+B2</f>
+        <v>40</v>
+      </c>
+      <c r="E2" s="6">
+        <f>-1*B1+B3</f>
+        <v>-10</v>
+      </c>
+      <c r="F2" s="6">
+        <f>1*B1+B4</f>
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="str">
+        <f>CONCATENATE(C2," ",D2," ",E2," ",F2)</f>
+        <v>v 40 -10 10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
         <f>1*B1+B2</f>
         <v>60</v>
       </c>
-      <c r="F1" s="1">
+      <c r="E3" s="6">
+        <f>-1*B1+B3</f>
+        <v>-10</v>
+      </c>
+      <c r="F3" s="6">
+        <f>1*B1+B4</f>
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="str">
+        <f>CONCATENATE(C3," ",D3," ",E3," ",F3)</f>
+        <v>v 60 -10 10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
         <f>1*B1+B2</f>
         <v>60</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4">
-        <v>-8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="3">
-        <f>1+H1</f>
-        <v>-7</v>
-      </c>
-      <c r="K1" s="3">
-        <f>2+H1</f>
-        <v>-6</v>
-      </c>
-      <c r="L1" s="3">
-        <f>3+H1</f>
-        <v>-5</v>
-      </c>
-      <c r="M1" s="3">
-        <f>4+H1</f>
-        <v>-4</v>
-      </c>
-      <c r="O1" s="1" t="str">
-        <f>CONCATENATE(C1," ",D1," ",E1," ",F1)</f>
-        <v>v 40 60 60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>50</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E4" s="6">
+        <f>1*B1+B3</f>
+        <v>10</v>
+      </c>
+      <c r="F4" s="6">
+        <f>1*B1+B4</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f>CONCATENATE(C4," ",D4," ",E4," ",F4)</f>
+        <v>v 60 10 10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D5" s="6">
         <f>-1*B1+B2</f>
         <v>40</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E5" s="6">
+        <f>1*B1+B3</f>
+        <v>10</v>
+      </c>
+      <c r="F5" s="6">
+        <f>-1*B1+B4</f>
+        <v>-10</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f>CONCATENATE(C5," ",D5," ",E5," ",F5)</f>
+        <v>v 40 10 -10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
         <f>-1*B1+B2</f>
         <v>40</v>
       </c>
-      <c r="F2" s="1">
+      <c r="E6" s="6">
+        <f>-1*B1+B3</f>
+        <v>-10</v>
+      </c>
+      <c r="F6" s="6">
+        <f>-1*B1+B4</f>
+        <v>-10</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f>CONCATENATE(C6," ",D6," ",E6," ",F6)</f>
+        <v>v 40 -10 -10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
         <f>1*B1+B2</f>
         <v>60</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="3">
-        <f>8+H1</f>
+      <c r="E7" s="6">
+        <f>-1*B1+B3</f>
+        <v>-10</v>
+      </c>
+      <c r="F7" s="6">
+        <f>-1*B1+B4</f>
+        <v>-10</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f>CONCATENATE(C7," ",D7," ",E7," ",F7)</f>
+        <v>v 60 -10 -10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="3">
-        <f>7+H1</f>
-        <v>-1</v>
-      </c>
-      <c r="L2" s="3">
-        <f>6+H1</f>
-        <v>-2</v>
-      </c>
-      <c r="M2" s="3">
-        <f>5+H1</f>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="D8" s="6">
         <f>1*B1+B2</f>
         <v>60</v>
       </c>
-      <c r="E3" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="F3" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3">
-        <f>4+H1</f>
+      <c r="E8" s="6">
+        <f>1*B1+B3</f>
+        <v>10</v>
+      </c>
+      <c r="F8" s="6">
+        <f>-1*B1+B4</f>
+        <v>-10</v>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f>CONCATENATE(C8," ",D8," ",E8," ",F8)</f>
+        <v>v 60 10 -10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f>CONCATENATE(C9," ",D9)</f>
+        <v>g FaceIndexReverse</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f>CONCATENATE(C10," ",D10)</f>
+        <v>usemtl red</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <f>1+B11</f>
+        <v>-8</v>
+      </c>
+      <c r="E11" s="3">
+        <f>2+B11</f>
+        <v>-7</v>
+      </c>
+      <c r="F11" s="3">
+        <f>3+B11</f>
+        <v>-6</v>
+      </c>
+      <c r="G11" s="3">
+        <f>4+B11</f>
+        <v>-5</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f>CONCATENATE(C11," ",D11," ",E11," ",F11," ",G11)</f>
+        <v>f -8 -7 -6 -5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="C12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <f>8+B11</f>
+        <v>-1</v>
+      </c>
+      <c r="E12" s="3">
+        <f>7+B11</f>
+        <v>-2</v>
+      </c>
+      <c r="F12" s="3">
+        <f>6+B11</f>
+        <v>-3</v>
+      </c>
+      <c r="G12" s="3">
+        <f>5+B11</f>
         <v>-4</v>
       </c>
-      <c r="K3" s="3">
-        <f>3+H1</f>
+      <c r="H12" s="1" t="str">
+        <f>CONCATENATE(C12," ",D12," ",E12," ",F12," ",G12)</f>
+        <v>f -1 -2 -3 -4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="C13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <f>4+B11</f>
         <v>-5</v>
       </c>
-      <c r="L3" s="3">
-        <f>7+H1</f>
+      <c r="E13" s="3">
+        <f>3+B11</f>
+        <v>-6</v>
+      </c>
+      <c r="F13" s="3">
+        <f>7+B11</f>
+        <v>-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f>8+B11</f>
         <v>-1</v>
       </c>
-      <c r="M3" s="3">
-        <f>8+H1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="E4" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="F4" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="3">
-        <f>5+H1</f>
+      <c r="H13" s="1" t="str">
+        <f>CONCATENATE(C13," ",D13," ",E13," ",F13," ",G13)</f>
+        <v>f -5 -6 -2 -1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="C14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <f>5+B11</f>
+        <v>-4</v>
+      </c>
+      <c r="E14" s="3">
+        <f>1+B11</f>
+        <v>-8</v>
+      </c>
+      <c r="F14" s="3">
+        <f>4+B11</f>
+        <v>-5</v>
+      </c>
+      <c r="G14" s="3">
+        <f>8+B11</f>
+        <v>-1</v>
+      </c>
+      <c r="H14" s="1" t="str">
+        <f t="shared" ref="H14:H16" si="0">CONCATENATE(C14," ",D14," ",E14," ",F14," ",G14)</f>
+        <v>f -4 -8 -5 -1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="C15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <f>5+B11</f>
+        <v>-4</v>
+      </c>
+      <c r="E15" s="3">
+        <f>6+B11</f>
         <v>-3</v>
       </c>
-      <c r="K4" s="3">
-        <f>1+H1</f>
+      <c r="F15" s="3">
+        <f>2+B11</f>
         <v>-7</v>
       </c>
-      <c r="L4" s="3">
-        <f>4+H1</f>
-        <v>-4</v>
-      </c>
-      <c r="M4" s="3">
-        <f>8+H1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="E5" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="F5" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="3">
-        <f>5+H1</f>
+      <c r="G15" s="3">
+        <f>1+B11</f>
+        <v>-8</v>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>f -4 -3 -7 -8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="C16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <f>2+B11</f>
+        <v>-7</v>
+      </c>
+      <c r="E16" s="3">
+        <f>6+B11</f>
         <v>-3</v>
       </c>
-      <c r="K5" s="3">
-        <f>6+H1</f>
+      <c r="F16" s="3">
+        <f>7+B11</f>
         <v>-2</v>
       </c>
-      <c r="L5" s="3">
-        <f>2+H1</f>
+      <c r="G16" s="3">
+        <f>3+B11</f>
         <v>-6</v>
       </c>
-      <c r="M5" s="3">
-        <f>1+H1</f>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="E6" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="F6" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="3">
-        <f>2+H1</f>
-        <v>-6</v>
-      </c>
-      <c r="K6" s="3">
-        <f>6+H1</f>
-        <v>-2</v>
-      </c>
-      <c r="L6" s="3">
-        <f>7+H1</f>
-        <v>-1</v>
-      </c>
-      <c r="M6" s="3">
-        <f>3+H1</f>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="E7" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-      <c r="F7" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="E8" s="1">
-        <f>1*B1+B2</f>
-        <v>60</v>
-      </c>
-      <c r="F8" s="1">
-        <f>-1*B1+B2</f>
-        <v>40</v>
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>f -7 -3 -2 -6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>